<commit_message>
"Sweatshirts and fleece" back to "sweatshirts"
</commit_message>
<xml_diff>
--- a/filters/db/apparel.xlsx
+++ b/filters/db/apparel.xlsx
@@ -121,9 +121,6 @@
     <t>t-shirts</t>
   </si>
   <si>
-    <t>sweatshirts &amp; fleece</t>
-  </si>
-  <si>
     <t>pants</t>
   </si>
   <si>
@@ -151,10 +148,13 @@
     <t>infant</t>
   </si>
   <si>
-    <t>Sweatshirts and Fleece</t>
-  </si>
-  <si>
     <t>Women's</t>
+  </si>
+  <si>
+    <t>Sweatshirts</t>
+  </si>
+  <si>
+    <t>sweatshirts</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -688,7 +688,7 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -711,7 +711,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -734,7 +734,7 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -757,7 +757,7 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -780,7 +780,7 @@
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -803,7 +803,7 @@
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -826,7 +826,7 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -849,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
@@ -872,7 +872,7 @@
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
accessories cat -> novelties & accessories
Name of filter and category was changed and needed to be updated
wherever used.
</commit_message>
<xml_diff>
--- a/filters/db/apparel.xlsx
+++ b/filters/db/apparel.xlsx
@@ -91,9 +91,6 @@
     <t>Hats</t>
   </si>
   <si>
-    <t>Accessories and Novelties</t>
-  </si>
-  <si>
     <t>Men's</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>sweatshirts</t>
+  </si>
+  <si>
+    <t>Novelties and Accessories</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,13 +590,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -613,13 +613,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -630,19 +630,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -659,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -682,13 +682,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -705,13 +705,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -722,19 +722,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -745,19 +745,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -768,19 +768,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -791,19 +791,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -814,19 +814,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -837,19 +837,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
@@ -860,19 +860,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
apparel merchandise category images / version
</commit_message>
<xml_diff>
--- a/filters/db/apparel.xlsx
+++ b/filters/db/apparel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -113,52 +113,55 @@
     <t>size_gender</t>
   </si>
   <si>
-    <t>shorts</t>
-  </si>
-  <si>
-    <t>t-shirts</t>
-  </si>
-  <si>
-    <t>pants</t>
-  </si>
-  <si>
-    <t>hats</t>
-  </si>
-  <si>
-    <t>novelties &amp; accessories</t>
-  </si>
-  <si>
-    <t>adult</t>
-  </si>
-  <si>
-    <t>womens</t>
-  </si>
-  <si>
-    <t>kids</t>
-  </si>
-  <si>
-    <t>youth</t>
-  </si>
-  <si>
-    <t>toddler</t>
-  </si>
-  <si>
-    <t>infant</t>
-  </si>
-  <si>
     <t>Women's</t>
   </si>
   <si>
     <t>Sweatshirts</t>
   </si>
   <si>
-    <t>sweatshirts</t>
-  </si>
-  <si>
     <t>Novelties and Accessories</t>
   </si>
   <si>
     <t xml:space="preserve">1. Shorts, T-shirts, etc. or Men's, Women's, etc. need to have the website_filter/size_gender attrib swapped removed respectively (easier to build w/ both and remove one manually) until json build can be edited to account for this special circumstance. </t>
+  </si>
+  <si>
+    <t>cat_images/shorts_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/tshirts_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/sweatshirts_apparel_merchandise.jpgs</t>
+  </si>
+  <si>
+    <t>cat_images/jerseys_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/pants_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/hats_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/novelties_accessories.jpgs</t>
+  </si>
+  <si>
+    <t>cat_images/mens_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/womens_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/kids_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/youth_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/toddler_apparel_merchandise.jpg</t>
+  </si>
+  <si>
+    <t>cat_images/infant_apparel_merchandise.jpg</t>
   </si>
 </sst>
 </file>
@@ -512,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +606,7 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -626,7 +629,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -637,7 +640,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -649,7 +652,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -672,7 +675,7 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -695,7 +698,7 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -718,7 +721,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -729,7 +732,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -741,7 +744,7 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -764,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -775,7 +778,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -787,7 +790,7 @@
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -810,7 +813,7 @@
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -833,7 +836,7 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -856,7 +859,7 @@
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
@@ -879,7 +882,7 @@
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
@@ -907,7 +910,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="381.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>